<commit_message>
Updated the CMS tab in the excel file for new test atoms for existing test cases.
</commit_message>
<xml_diff>
--- a/docs/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/docs/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\piv-conformance\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C936CACE-5CC5-46E6-992A-C1B0D84C4EF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9EAC4-7585-464B-8B50-98A1641D1EC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="195" windowWidth="28650" windowHeight="15975" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="1173">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3041,15 +3041,9 @@
     <t>CMS_Test_4</t>
   </si>
   <si>
-    <t>Verify digestAlgorithms attribute is present and algorithm is present and consistent with signature algorithm</t>
-  </si>
-  <si>
     <t>CMS_Test_5</t>
   </si>
   <si>
-    <t>Ensure encapsulated content is absent and eContentType is id-piv-CHUIDSecurityContent in encapContentInfo</t>
-  </si>
-  <si>
     <t>CMS_Test_6</t>
   </si>
   <si>
@@ -3071,9 +3065,6 @@
     <t>CMS_Test_9</t>
   </si>
   <si>
-    <t>Ensure that the Issuer and Serial in the signer info corresponds to the issuer and serial values in the signer certificate</t>
-  </si>
-  <si>
     <t>CMS.11</t>
   </si>
   <si>
@@ -3086,9 +3077,6 @@
     <t>CMS_Test_12</t>
   </si>
   <si>
-    <t>Validate that signed attributes includes pivSigner-DN and that this DN matches the one asserted in signing certificate</t>
-  </si>
-  <si>
     <t>CMS_Test_13</t>
   </si>
   <si>
@@ -3128,15 +3116,9 @@
     <t>CMS_Test_17</t>
   </si>
   <si>
-    <t>Confirm that signed attributes include pivFASC-N and entryUUID attributes and that they match FASC-N and GUID read from CHUID container</t>
-  </si>
-  <si>
     <t>2.16.840.1.101.3.6.6, 1.3.6.1.1.16.4</t>
   </si>
   <si>
-    <t>OIDs for piv-FASC-N, OID for entryUUID</t>
-  </si>
-  <si>
     <t>CMS_Test_18</t>
   </si>
   <si>
@@ -3471,6 +3453,105 @@
   </si>
   <si>
     <t>PKIX_Test_26</t>
+  </si>
+  <si>
+    <t>CMS.24</t>
+  </si>
+  <si>
+    <t>CMS_Test_24</t>
+  </si>
+  <si>
+    <t>CMS.4_Extn Verify digest algorithm is present</t>
+  </si>
+  <si>
+    <t>CMS.25</t>
+  </si>
+  <si>
+    <t>CMS_Test_25</t>
+  </si>
+  <si>
+    <t>CMS.4_Extn Verify that digest algorithm is consistent with the signature algorithm</t>
+  </si>
+  <si>
+    <t>Verify digestAlgorithms attribute is present</t>
+  </si>
+  <si>
+    <t>CMS.26</t>
+  </si>
+  <si>
+    <t>CMS_Test_26</t>
+  </si>
+  <si>
+    <t>CMS.5_Extn Ensure eContentType is id-piv-CHUIDSecurityContent in encapContentInfo</t>
+  </si>
+  <si>
+    <t>Ensure encapsulated content is absent</t>
+  </si>
+  <si>
+    <t>CMS.27</t>
+  </si>
+  <si>
+    <t>CMS_Test_27</t>
+  </si>
+  <si>
+    <t>CMS.9_Extn Ensure that the Serial in the signer info corresponds to the serial value in the signer certificate</t>
+  </si>
+  <si>
+    <t>Ensure that the Issuer in the signer info corresponds to the issuer value in the signer certificate</t>
+  </si>
+  <si>
+    <t>CMS.28</t>
+  </si>
+  <si>
+    <t>CMS_Test_28</t>
+  </si>
+  <si>
+    <t>CMS.12_Extn Validate that signed attribute pivSigner-DN matches the one asserted in signing certificate</t>
+  </si>
+  <si>
+    <t>Validate that signed attributes includes pivSigner-DN</t>
+  </si>
+  <si>
+    <t>CMS.29</t>
+  </si>
+  <si>
+    <t>CMS_Test_29</t>
+  </si>
+  <si>
+    <t>CMS.30</t>
+  </si>
+  <si>
+    <t>CMS_Test_30</t>
+  </si>
+  <si>
+    <t>CMS.31</t>
+  </si>
+  <si>
+    <t>CMS_Test_31</t>
+  </si>
+  <si>
+    <t>CMS.17_Extn Confirm that signed attributes include entryUUID attribute</t>
+  </si>
+  <si>
+    <t>CMS.17_Extn Confirm that signed attribute pivFASC-N matches FASC-N read from CHUID container</t>
+  </si>
+  <si>
+    <t>CMS.17_Extn Confirm that signed attribute entryUUID matches GUID read from CHUID container</t>
+  </si>
+  <si>
+    <t>Confirm that signed attributes include pivFASC-N attribute</t>
+  </si>
+  <si>
+    <t>2.16.840.1.101.3.6.6</t>
+  </si>
+  <si>
+    <t>OID for piv-FASC-N</t>
+  </si>
+  <si>
+    <t>1.3.6.1.1.16.4</t>
+  </si>
+  <si>
+    <t>OID for entryUUID; CMS.29 and CMS.17 could be the same test case with different input parameters</t>
   </si>
 </sst>
 </file>
@@ -7909,8 +7990,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B205" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209"/>
+    <sheetView topLeftCell="B214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F235" sqref="F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11038,7 +11119,7 @@
         <v>373</v>
       </c>
       <c r="D194" s="42" t="s">
-        <v>1127</v>
+        <v>1121</v>
       </c>
       <c r="E194" s="11"/>
       <c r="F194" s="3">
@@ -11149,11 +11230,11 @@
         <v>385</v>
       </c>
       <c r="C201" s="41" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="D201" s="3"/>
       <c r="E201" s="11" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="F201" s="48" t="s">
         <v>273</v>
@@ -11171,7 +11252,7 @@
       </c>
       <c r="D202" s="3"/>
       <c r="E202" s="11" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="F202" s="48" t="s">
         <v>273</v>
@@ -11185,7 +11266,7 @@
         <v>389</v>
       </c>
       <c r="C203" s="42" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="D203" s="3"/>
       <c r="E203" s="11"/>
@@ -11250,7 +11331,7 @@
         <v>399</v>
       </c>
       <c r="D207" s="42" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="E207" s="11"/>
       <c r="F207" s="3">
@@ -13054,7 +13135,7 @@
         <v>594</v>
       </c>
       <c r="D321" s="5" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="E321" s="11"/>
       <c r="F321" s="3" t="s">
@@ -13085,12 +13166,12 @@
         <v>599</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="D323" s="5"/>
       <c r="E323" s="11"/>
       <c r="F323" s="3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -13248,7 +13329,7 @@
         <v>627</v>
       </c>
       <c r="D333" s="7" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E333" s="11"/>
       <c r="F333" s="3" t="s">
@@ -13270,7 +13351,7 @@
         <v>630</v>
       </c>
       <c r="F334" s="3" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="335" spans="1:6">
@@ -13298,7 +13379,7 @@
         <v>594</v>
       </c>
       <c r="D336" s="5" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="E336" s="11"/>
       <c r="F336" s="42" t="s">
@@ -13318,7 +13399,7 @@
       <c r="D337" s="5"/>
       <c r="E337" s="24"/>
       <c r="F337" s="42" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="338" spans="1:6">
@@ -13350,7 +13431,7 @@
       <c r="D339" s="27"/>
       <c r="E339" s="11"/>
       <c r="F339" s="3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="340" spans="1:6">
@@ -13368,7 +13449,7 @@
         <v>642</v>
       </c>
       <c r="F340" s="3" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="341" spans="1:6">
@@ -13600,7 +13681,7 @@
         <v>627</v>
       </c>
       <c r="D355" s="8" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E355" s="11"/>
       <c r="F355" s="3" t="s">
@@ -13622,7 +13703,7 @@
         <v>630</v>
       </c>
       <c r="F356" s="42" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -13650,7 +13731,7 @@
         <v>594</v>
       </c>
       <c r="D358" s="27" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="E358" s="11"/>
       <c r="F358" s="3" t="s">
@@ -13670,7 +13751,7 @@
       <c r="D359" s="27"/>
       <c r="E359" s="24"/>
       <c r="F359" s="3" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="360" spans="1:6">
@@ -13702,7 +13783,7 @@
       <c r="D361" s="7"/>
       <c r="E361" s="11"/>
       <c r="F361" s="3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="362" spans="1:6">
@@ -13720,7 +13801,7 @@
         <v>642</v>
       </c>
       <c r="F362" s="42" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="363" spans="1:6">
@@ -13952,7 +14033,7 @@
         <v>627</v>
       </c>
       <c r="D377" s="8" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E377" s="11"/>
       <c r="F377" s="3" t="s">
@@ -13974,7 +14055,7 @@
         <v>630</v>
       </c>
       <c r="F378" s="42" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="379" spans="1:6">
@@ -14002,7 +14083,7 @@
         <v>594</v>
       </c>
       <c r="D380" s="27" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="E380" s="11"/>
       <c r="F380" s="3" t="s">
@@ -14022,7 +14103,7 @@
       <c r="D381" s="27"/>
       <c r="E381" s="24"/>
       <c r="F381" s="3" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="382" spans="1:6">
@@ -14054,7 +14135,7 @@
       <c r="D383" s="7"/>
       <c r="E383" s="11"/>
       <c r="F383" s="3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="384" spans="1:6">
@@ -14072,7 +14153,7 @@
         <v>642</v>
       </c>
       <c r="F384" s="42" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="385" spans="1:6">
@@ -14528,7 +14609,7 @@
         <v>627</v>
       </c>
       <c r="D413" s="8" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E413" s="11"/>
       <c r="F413" s="3" t="s">
@@ -14550,7 +14631,7 @@
         <v>630</v>
       </c>
       <c r="F414" s="42" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="415" spans="1:6">
@@ -14561,7 +14642,7 @@
         <v>753</v>
       </c>
       <c r="C415" s="13" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="D415" s="22"/>
       <c r="E415" s="11"/>
@@ -14582,7 +14663,7 @@
         <v>642</v>
       </c>
       <c r="F416" s="42" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="417" spans="1:6">
@@ -14810,7 +14891,7 @@
         <v>771</v>
       </c>
       <c r="D431" s="27" t="s">
-        <v>1133</v>
+        <v>1127</v>
       </c>
       <c r="E431" s="11"/>
       <c r="F431" s="3" t="s">
@@ -14846,7 +14927,7 @@
       <c r="D433" s="7"/>
       <c r="E433" s="11"/>
       <c r="F433" s="42" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="434" spans="1:6">
@@ -14922,7 +15003,7 @@
         <v>627</v>
       </c>
       <c r="D438" s="27" t="s">
-        <v>1130</v>
+        <v>1124</v>
       </c>
       <c r="E438" s="11"/>
       <c r="F438" s="3" t="s">
@@ -14942,7 +15023,7 @@
       <c r="D439" s="7"/>
       <c r="E439" s="11"/>
       <c r="F439" s="42" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="440" spans="1:6">
@@ -14970,7 +15051,7 @@
         <v>594</v>
       </c>
       <c r="D441" s="8" t="s">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="E441" s="11"/>
       <c r="F441" s="3" t="s">
@@ -15022,7 +15103,7 @@
       <c r="D444" s="3"/>
       <c r="E444" s="11"/>
       <c r="F444" s="3" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="445" spans="1:6">
@@ -15038,7 +15119,7 @@
       <c r="D445" s="3"/>
       <c r="E445" s="11"/>
       <c r="F445" s="42" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
     </row>
   </sheetData>
@@ -15199,7 +15280,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -15948,7 +16031,7 @@
         <v>281</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>863</v>
@@ -15967,7 +16050,7 @@
         <v>278</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>864</v>
@@ -15986,7 +16069,7 @@
         <v>270</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>866</v>
@@ -16005,7 +16088,7 @@
         <v>267</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>868</v>
@@ -16024,7 +16107,7 @@
         <v>276</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1116</v>
+        <v>1110</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>870</v>
@@ -16052,8 +16135,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:IV49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -16608,16 +16691,16 @@
     </row>
     <row r="16" spans="1:256" ht="31.5" customHeight="1">
       <c r="A16" s="45" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>873</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="3" t="s">
@@ -16627,16 +16710,16 @@
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
       <c r="A17" s="45" t="s">
-        <v>1117</v>
+        <v>1111</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>873</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="3"/>
@@ -16653,7 +16736,7 @@
         <v>907</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>1128</v>
+        <v>1122</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="3" t="s">
@@ -17229,10 +17312,10 @@
         <v>873</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="E49" s="50"/>
       <c r="F49" s="50"/>
@@ -17499,9 +17582,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:IV23"/>
+  <dimension ref="A1:IV36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:G31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -17608,7 +17693,7 @@
         <v>1001</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>1002</v>
+        <v>1146</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -17624,10 +17709,10 @@
         <v>994</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1004</v>
+        <v>1150</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
@@ -17643,10 +17728,10 @@
         <v>994</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
@@ -17662,10 +17747,10 @@
         <v>994</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
@@ -17681,10 +17766,10 @@
         <v>994</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
@@ -17700,10 +17785,10 @@
         <v>994</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>1012</v>
+        <v>1154</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
@@ -17713,16 +17798,16 @@
     </row>
     <row r="11" spans="1:7" ht="47.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>994</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
@@ -17738,10 +17823,10 @@
         <v>994</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>1017</v>
+        <v>1158</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
@@ -17757,19 +17842,19 @@
         <v>994</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>798</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.5" customHeight="1">
@@ -17780,10 +17865,10 @@
         <v>994</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
@@ -17799,19 +17884,19 @@
         <v>994</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>798</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="47.25" customHeight="1">
@@ -17822,10 +17907,10 @@
         <v>994</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
@@ -17841,19 +17926,19 @@
         <v>994</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1031</v>
+        <v>1168</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>1032</v>
+        <v>1169</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>798</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>1033</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="31.5" customHeight="1">
@@ -17864,7 +17949,7 @@
         <v>994</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>536</v>
@@ -17883,7 +17968,7 @@
         <v>994</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>539</v>
@@ -17902,10 +17987,10 @@
         <v>994</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
@@ -17921,10 +18006,10 @@
         <v>994</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
@@ -17940,10 +18025,10 @@
         <v>994</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
@@ -17959,7 +18044,7 @@
         <v>994</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>548</v>
@@ -17967,6 +18052,191 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="31.5">
+      <c r="A24" s="5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="31.5" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" ht="31.5" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="47.25">
+      <c r="A27" s="5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" ht="47.25">
+      <c r="A28" s="5" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" ht="63">
+      <c r="A29" s="5" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="31.5">
+      <c r="A30" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" ht="47.25">
+      <c r="A31" s="5" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>994</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="31.5" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="31.5" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -18021,19 +18291,19 @@
     </row>
     <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>1046</v>
+        <v>1040</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>798</v>
@@ -18042,19 +18312,19 @@
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>1048</v>
+        <v>1042</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1050</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>1047</v>
+        <v>1041</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>798</v>
@@ -18063,19 +18333,19 @@
     </row>
     <row r="4" spans="1:7" ht="31.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>798</v>
@@ -18388,23 +18658,23 @@
     </row>
     <row r="2" spans="1:256" ht="31.5" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
@@ -18412,13 +18682,13 @@
         <v>654</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33" t="s">
@@ -18431,13 +18701,13 @@
         <v>581</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>1055</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>1061</v>
-      </c>
       <c r="D4" s="33" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="E4" s="34"/>
       <c r="F4" s="33" t="s">
@@ -18450,13 +18720,13 @@
         <v>584</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>1063</v>
+        <v>1057</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>1064</v>
+        <v>1058</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="33" t="s">
@@ -18469,13 +18739,13 @@
         <v>587</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>1065</v>
+        <v>1059</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>1066</v>
+        <v>1060</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="33" t="s">
@@ -18488,22 +18758,22 @@
         <v>590</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>1067</v>
+        <v>1061</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1069</v>
+        <v>1063</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>1070</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="31.5" customHeight="1">
@@ -18511,13 +18781,13 @@
         <v>595</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>1071</v>
+        <v>1065</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>1072</v>
+        <v>1066</v>
       </c>
       <c r="E8" s="34"/>
       <c r="F8" s="33" t="s">
@@ -18530,13 +18800,13 @@
         <v>598</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>1073</v>
+        <v>1067</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>1074</v>
+        <v>1068</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="33" t="s">
@@ -18549,13 +18819,13 @@
         <v>601</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>1075</v>
+        <v>1069</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>1076</v>
+        <v>1070</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="33" t="s">
@@ -18568,13 +18838,13 @@
         <v>604</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>1078</v>
+        <v>1072</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="33" t="s">
@@ -18587,10 +18857,10 @@
         <v>607</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>1079</v>
+        <v>1073</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>606</v>
@@ -18606,22 +18876,22 @@
         <v>610</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>1080</v>
+        <v>1074</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>1081</v>
+        <v>1075</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>1032</v>
+        <v>1027</v>
       </c>
       <c r="F13" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>1082</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="14" spans="1:256" ht="31.5" customHeight="1">
@@ -18629,22 +18899,22 @@
         <v>620</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>1083</v>
+        <v>1077</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1085</v>
+        <v>1079</v>
       </c>
       <c r="F14" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G14" s="33" t="s">
-        <v>1086</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="15" spans="1:256" ht="31.5" customHeight="1">
@@ -18652,13 +18922,13 @@
         <v>623</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>1087</v>
+        <v>1081</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>1088</v>
+        <v>1082</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="33" t="s">
@@ -18671,13 +18941,13 @@
         <v>657</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>1089</v>
+        <v>1083</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>1090</v>
+        <v>1084</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="33" t="s">
@@ -18687,16 +18957,16 @@
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
       <c r="A17" s="33" t="s">
-        <v>1091</v>
+        <v>1085</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>1092</v>
+        <v>1086</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>1093</v>
+        <v>1087</v>
       </c>
       <c r="E17" s="34"/>
       <c r="F17" s="33" t="s">
@@ -18709,13 +18979,13 @@
         <v>691</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>1094</v>
+        <v>1088</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>1095</v>
+        <v>1089</v>
       </c>
       <c r="E18" s="34"/>
       <c r="F18" s="33" t="s">
@@ -18725,25 +18995,25 @@
     </row>
     <row r="19" spans="1:7" ht="31.5" customHeight="1">
       <c r="A19" s="33" t="s">
-        <v>1096</v>
+        <v>1090</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>1099</v>
+        <v>1093</v>
       </c>
       <c r="F19" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>1100</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
@@ -18751,13 +19021,13 @@
         <v>728</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>1101</v>
+        <v>1095</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>1102</v>
+        <v>1096</v>
       </c>
       <c r="E20" s="34"/>
       <c r="F20" s="33" t="s">
@@ -18770,56 +19040,56 @@
         <v>731</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="F21" s="33" t="s">
         <v>798</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>1106</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1">
       <c r="A22" s="34" t="s">
-        <v>1107</v>
+        <v>1101</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>1108</v>
+        <v>1102</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>1109</v>
+        <v>1103</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>817</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>1111</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.5">
       <c r="A23" s="50" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="D23" s="50" t="s">
         <v>635</v>
@@ -18830,13 +19100,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="50" t="s">
-        <v>1135</v>
+        <v>1129</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="D24" s="50" t="s">
         <v>639</v>
@@ -18847,13 +19117,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="50" t="s">
-        <v>1129</v>
+        <v>1123</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="D25" s="50" t="s">
         <v>629</v>
@@ -18864,13 +19134,13 @@
     </row>
     <row r="26" spans="1:7" ht="31.5">
       <c r="A26" s="50" t="s">
-        <v>1132</v>
+        <v>1126</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="D26" s="50" t="s">
         <v>641</v>
@@ -18881,13 +19151,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="51" t="s">
-        <v>1134</v>
+        <v>1128</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="C27" s="43" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="D27" s="50" t="s">
         <v>774</v>
@@ -19201,20 +19471,20 @@
         <v>273</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1112</v>
+        <v>1106</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1113</v>
+        <v>1107</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>1114</v>
+        <v>1108</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
         <v>798</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>1115</v>
+        <v>1109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>